<commit_message>
Update: Add line-of-sight test for SX1280 module
</commit_message>
<xml_diff>
--- a/Documents/SX1280/Test/TestLog.xlsx
+++ b/Documents/SX1280/Test/TestLog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\KLTN\Documents\SX1280\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7411BFF-7F79-414D-AB10-256486048980}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58F132B-FF83-4540-B7F0-9D20D77D76DD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="2892" xr2:uid="{3D1FB1CC-A3A4-4ADA-877A-DDD423325106}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>No.</t>
   </si>
@@ -82,6 +82,39 @@
     <t>- SLAVE was put int room E6.1
 - MASTER is near USSH (see in picture)
 - Testing in heterogeneous environment (not Line of Sight)
+- MASTER &amp; SLAVE are set at highest ranging precision (Max BW 1600, Max SF SF10)</t>
+  </si>
+  <si>
+    <t>.\RangingResult\Test_4_5_6\</t>
+  </si>
+  <si>
+    <t>- High error
+- Ranging result average was ~147.23m while real distance was ~394.74m</t>
+  </si>
+  <si>
+    <t>- High error
+- Ranging result average was ~485.58m while real distance was ~704.4m</t>
+  </si>
+  <si>
+    <t>- High error
+- Ranging result average was ~165.43m while real distance was ~374.85m</t>
+  </si>
+  <si>
+    <t>- SLAVE on roof of E building
+- MASTER is near USSH main gate (see in picture)
+- Line of Sight
+- MASTER &amp; SLAVE are set at highest ranging precision (Max BW 1600, Max SF SF10)</t>
+  </si>
+  <si>
+    <t>- SLAVE on roof of E building
+- MASTER is near HCMUS (see in picture)
+- Line of Sight
+- MASTER &amp; SLAVE are set at highest ranging precision (Max BW 1600, Max SF SF10)</t>
+  </si>
+  <si>
+    <t>- SLAVE on roof of E building
+- MASTER is near Suoi Tien Park's Gate (see in picture)
+- Line of Sight
 - MASTER &amp; SLAVE are set at highest ranging precision (Max BW 1600, Max SF SF10)</t>
   </si>
 </sst>
@@ -139,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -199,12 +232,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,17 +288,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -553,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29024CB3-52ED-4515-94B7-4A1E3F17D873}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +677,7 @@
       <c r="F2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -630,8 +697,8 @@
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -649,41 +716,67 @@
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="8"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>43258</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.71193287037037034</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>43258</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.71767361111111105</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="3">
+        <v>43258</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.73249999999999993</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
@@ -785,9 +878,10 @@
       <c r="G16" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G2:G4"/>
+  <mergeCells count="3">
     <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A738F118-AC84-42C3-8A20-6D96D7779EE8}"/>

</xml_diff>